<commit_message>
updated assessment and made many changes
</commit_message>
<xml_diff>
--- a/runs/ControlFile.xlsx
+++ b/runs/ControlFile.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11009"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jim/_mymods/ebswp/runs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90B50628-73FB-3346-89B3-B52358935BB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1C0B273-8EC4-A54A-9994-730231E84D60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{6E3F6ADE-442B-FE4B-9381-B027FAEA0EB9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -529,9 +530,6 @@
     <t>Switch for BTS sel penalty type (on lnsel, or params)</t>
   </si>
   <si>
-    <t>Reserved for larval drift penalty …</t>
-  </si>
-  <si>
     <t>#DoCovBTS</t>
   </si>
   <si>
@@ -731,6 +729,9 @@
   </si>
   <si>
     <t>#switch_multispecies_fucntional_response</t>
+  </si>
+  <si>
+    <t>Set 2018 YC to mean of 2012 and 2013 for projections</t>
   </si>
 </sst>
 </file>
@@ -808,7 +809,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -817,7 +818,6 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1135,8 +1135,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93CF87E0-DDDF-C74A-A096-73DD518D7BF1}">
   <dimension ref="A1:G178"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="179" workbookViewId="0">
-      <selection activeCell="A12" activeCellId="1" sqref="B15 A12"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A117" zoomScale="179" workbookViewId="0">
+      <selection activeCell="C156" sqref="C156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1152,7 +1152,7 @@
         <v>#DoCovBTS</v>
       </c>
       <c r="B1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C1" t="s">
         <v>31</v>
@@ -1182,7 +1182,7 @@
         <v>#SrType</v>
       </c>
       <c r="B3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C3" t="s">
         <v>31</v>
@@ -1212,7 +1212,7 @@
         <v>#Do_Combined</v>
       </c>
       <c r="B5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C5" t="s">
         <v>31</v>
@@ -1242,7 +1242,7 @@
         <v>#use_age_err</v>
       </c>
       <c r="B7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C7" t="s">
         <v>31</v>
@@ -1272,7 +1272,7 @@
         <v>#use_age1_eit</v>
       </c>
       <c r="B9" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C9" t="s">
         <v>31</v>
@@ -1302,7 +1302,7 @@
         <v>#age1_sigma_eit</v>
       </c>
       <c r="B11" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C11" t="s">
         <v>31</v>
@@ -1332,7 +1332,7 @@
         <v>#use_endyr_len</v>
       </c>
       <c r="B13" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C13" t="s">
         <v>31</v>
@@ -1362,7 +1362,7 @@
         <v>#use_popwts_ssb</v>
       </c>
       <c r="B15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C15" t="s">
         <v>31</v>
@@ -1392,7 +1392,7 @@
         <v>#natmortprior</v>
       </c>
       <c r="B17" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C17" t="s">
         <v>31</v>
@@ -1419,7 +1419,7 @@
         <v>#cvnatmortprior</v>
       </c>
       <c r="B19" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C19" t="s">
         <v>31</v>
@@ -1446,7 +1446,7 @@
         <v>#natmort_in</v>
       </c>
       <c r="B21" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C21" t="s">
         <v>31</v>
@@ -1644,7 +1644,7 @@
         <v>#q_all_prior</v>
       </c>
       <c r="B37" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C37" t="s">
         <v>31</v>
@@ -1671,7 +1671,7 @@
         <v>#q_all_sigma</v>
       </c>
       <c r="B39" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C39" t="s">
         <v>31</v>
@@ -1698,7 +1698,7 @@
         <v>#q_bts_prior</v>
       </c>
       <c r="B41" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C41" t="s">
         <v>31</v>
@@ -1725,7 +1725,7 @@
         <v>#q_bts_sigma</v>
       </c>
       <c r="B43" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C43" t="s">
         <v>31</v>
@@ -1752,7 +1752,7 @@
         <v>#sigrprior</v>
       </c>
       <c r="B45" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C45" t="s">
         <v>31</v>
@@ -1779,7 +1779,7 @@
         <v>#cvsigrprior</v>
       </c>
       <c r="B47" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C47" t="s">
         <v>31</v>
@@ -1806,7 +1806,7 @@
         <v>#phase_sigr</v>
       </c>
       <c r="B49" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C49" t="s">
         <v>31</v>
@@ -1833,7 +1833,7 @@
         <v>#steepnessprior</v>
       </c>
       <c r="B51" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C51" t="s">
         <v>31</v>
@@ -1860,7 +1860,7 @@
         <v>#cvsteepnessprior</v>
       </c>
       <c r="B53" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C53" t="s">
         <v>31</v>
@@ -1887,7 +1887,7 @@
         <v>#phase_steepness</v>
       </c>
       <c r="B55" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C55" t="s">
         <v>31</v>
@@ -1914,7 +1914,7 @@
         <v>#use_spr_msy_pen</v>
       </c>
       <c r="B57" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C57" t="s">
         <v>31</v>
@@ -1944,7 +1944,7 @@
         <v>#sigma_spr_msy</v>
       </c>
       <c r="B59" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C59" t="s">
         <v>31</v>
@@ -1974,7 +1974,7 @@
         <v>#use_last_eit_ac</v>
       </c>
       <c r="B61" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C61" t="s">
         <v>31</v>
@@ -2004,7 +2004,7 @@
         <v>#nyrs_sel_avg</v>
       </c>
       <c r="B63" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C63" t="s">
         <v>31</v>
@@ -2040,7 +2040,7 @@
         <v>#do_bts_bio</v>
       </c>
       <c r="B65" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C65" t="s">
         <v>31</v>
@@ -2070,7 +2070,7 @@
         <v>#do_eit_bio</v>
       </c>
       <c r="B67" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C67" t="s">
         <v>31</v>
@@ -2100,7 +2100,7 @@
         <v>#srprior_a</v>
       </c>
       <c r="B69" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C69" t="s">
         <v>31</v>
@@ -2130,7 +2130,7 @@
         <v>#srprior_b</v>
       </c>
       <c r="B71" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C71" t="s">
         <v>31</v>
@@ -2160,7 +2160,7 @@
         <v>#nyrs_future;</v>
       </c>
       <c r="B73" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C73" t="s">
         <v>31</v>
@@ -2187,7 +2187,7 @@
         <v>#next_yrs_catch;</v>
       </c>
       <c r="B75" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C75" t="s">
         <v>31</v>
@@ -2220,7 +2220,7 @@
         <v>#nscen</v>
       </c>
       <c r="B77" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C77" t="s">
         <v>31</v>
@@ -2253,7 +2253,7 @@
         <v>#fixed_catch_fut2;</v>
       </c>
       <c r="B79" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C79" t="s">
         <v>31</v>
@@ -2280,7 +2280,7 @@
         <v>#fixed_catch_fut3;</v>
       </c>
       <c r="B81" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C81" t="s">
         <v>31</v>
@@ -2307,7 +2307,7 @@
         <v>#phase_F40;</v>
       </c>
       <c r="B83" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C83" t="s">
         <v>31</v>
@@ -2334,7 +2334,7 @@
         <v>#robust_phase</v>
       </c>
       <c r="B85" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C85" t="s">
         <v>31</v>
@@ -2361,7 +2361,7 @@
         <v>#eit_robust_phase</v>
       </c>
       <c r="B87" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C87" t="s">
         <v>31</v>
@@ -2388,7 +2388,7 @@
         <v>#eit_like_type</v>
       </c>
       <c r="B89" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C89" t="s">
         <v>31</v>
@@ -2418,7 +2418,7 @@
         <v>#phase_logist_fsh</v>
       </c>
       <c r="B91" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C91" t="s">
         <v>31</v>
@@ -2448,7 +2448,7 @@
         <v>#phase_logist_bts</v>
       </c>
       <c r="B93" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C93" t="s">
         <v>31</v>
@@ -2478,7 +2478,7 @@
         <v>#phase_seldevs_fsh</v>
       </c>
       <c r="B95" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C95" t="s">
         <v>31</v>
@@ -2508,7 +2508,7 @@
         <v>#phase_seldevs_bts</v>
       </c>
       <c r="B97" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C97" t="s">
         <v>31</v>
@@ -2538,7 +2538,7 @@
         <v>#phase_age1devs_bts</v>
       </c>
       <c r="B99" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C99" t="s">
         <v>31</v>
@@ -2568,7 +2568,7 @@
         <v>#phase_selcoffs_eit</v>
       </c>
       <c r="B101" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C101" t="s">
         <v>31</v>
@@ -2595,7 +2595,7 @@
         <v>#phase_selcoffs_eit_dev</v>
       </c>
       <c r="B103" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C103" t="s">
         <v>31</v>
@@ -2622,7 +2622,7 @@
         <v>#phase_natmort</v>
       </c>
       <c r="B105" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C105" t="s">
         <v>31</v>
@@ -2649,7 +2649,7 @@
         <v>#phase_q_bts</v>
       </c>
       <c r="B107" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C107" t="s">
         <v>31</v>
@@ -2679,7 +2679,7 @@
         <v>#phase_q_std_area</v>
       </c>
       <c r="B109" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C109" t="s">
         <v>31</v>
@@ -2706,7 +2706,7 @@
         <v>#phase_q_eit</v>
       </c>
       <c r="B111" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C111" t="s">
         <v>31</v>
@@ -2736,7 +2736,7 @@
         <v>#phase_bt</v>
       </c>
       <c r="B113" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C113" t="s">
         <v>31</v>
@@ -2766,7 +2766,7 @@
         <v>#phase_rec_devs</v>
       </c>
       <c r="B115" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C115" t="s">
         <v>31</v>
@@ -2796,7 +2796,7 @@
         <v>#phase_larv</v>
       </c>
       <c r="B117" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C117" t="s">
         <v>31</v>
@@ -2826,7 +2826,7 @@
         <v>#phase_sr</v>
       </c>
       <c r="B119" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C119" t="s">
         <v>31</v>
@@ -2856,7 +2856,7 @@
         <v>#wt_fut_phase</v>
       </c>
       <c r="B121" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C121" t="s">
         <v>31</v>
@@ -2886,7 +2886,7 @@
         <v>#last_age_sel_group_fsh</v>
       </c>
       <c r="B123" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C123" t="s">
         <v>31</v>
@@ -2913,7 +2913,7 @@
         <v>#last_age_sel_group_bts</v>
       </c>
       <c r="B125" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C125" t="s">
         <v>31</v>
@@ -2940,7 +2940,7 @@
         <v>#last_age_sel_group_eit</v>
       </c>
       <c r="B127" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C127" t="s">
         <v>31</v>
@@ -2967,7 +2967,7 @@
         <v>#ctrl_flag</v>
       </c>
       <c r="B129" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C129" t="s">
         <v>31</v>
@@ -3472,20 +3472,20 @@
     <row r="156" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>-3</v>
+        <v>1</v>
       </c>
       <c r="B156">
         <v>-3</v>
       </c>
       <c r="C156">
-        <v>-3</v>
+        <v>1</v>
       </c>
       <c r="E156">
         <f t="shared" si="3"/>
         <v>27</v>
       </c>
       <c r="F156" t="s">
-        <v>163</v>
+        <v>230</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.2">
@@ -3551,7 +3551,7 @@
         <v>#sel_dev_shift</v>
       </c>
       <c r="B160" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C160" t="s">
         <v>31</v>
@@ -3578,7 +3578,7 @@
         <v>#phase_coheff</v>
       </c>
       <c r="B162" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C162" t="s">
         <v>31</v>
@@ -3605,7 +3605,7 @@
         <v>#phase_yreff</v>
       </c>
       <c r="B164" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C164" t="s">
         <v>31</v>
@@ -3629,7 +3629,7 @@
     <row r="166" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A166" s="1"/>
       <c r="B166" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.2">
@@ -3641,7 +3641,7 @@
     <row r="168" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A168" s="1"/>
       <c r="B168" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.2">
@@ -3653,7 +3653,7 @@
     <row r="170" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A170" s="1"/>
       <c r="B170" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.2">
@@ -3665,7 +3665,7 @@
     <row r="172" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A172" s="1"/>
       <c r="B172" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.2">
@@ -3677,7 +3677,7 @@
     <row r="174" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A174" s="1"/>
       <c r="B174" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.2">
@@ -3688,15 +3688,12 @@
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A176" s="1"/>
-      <c r="B176" s="8"/>
-    </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A177" s="1"/>
-      <c r="B177" s="8"/>
-    </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A178" s="1"/>
-      <c r="B178" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3715,7 +3712,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
@@ -3725,7 +3722,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
@@ -3735,7 +3732,7 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
@@ -3745,7 +3742,7 @@
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
@@ -3755,7 +3752,7 @@
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
@@ -3765,7 +3762,7 @@
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
@@ -3775,7 +3772,7 @@
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
@@ -3785,7 +3782,7 @@
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
@@ -3795,7 +3792,7 @@
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
@@ -3805,7 +3802,7 @@
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
@@ -3815,7 +3812,7 @@
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
@@ -3895,7 +3892,7 @@
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
@@ -3905,7 +3902,7 @@
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
@@ -3915,7 +3912,7 @@
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
@@ -3925,7 +3922,7 @@
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
@@ -3935,7 +3932,7 @@
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
@@ -3945,7 +3942,7 @@
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
@@ -3955,7 +3952,7 @@
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
@@ -3965,7 +3962,7 @@
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
@@ -3975,7 +3972,7 @@
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
@@ -3985,7 +3982,7 @@
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
@@ -3995,7 +3992,7 @@
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
@@ -4005,7 +4002,7 @@
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
@@ -4015,7 +4012,7 @@
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
@@ -4025,7 +4022,7 @@
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
@@ -4035,7 +4032,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
@@ -4045,7 +4042,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
@@ -4055,7 +4052,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
@@ -4065,7 +4062,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
@@ -4075,7 +4072,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
@@ -4085,7 +4082,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
@@ -4095,7 +4092,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
@@ -4103,12 +4100,12 @@
         <v>8</v>
       </c>
       <c r="B78" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
@@ -4118,7 +4115,7 @@
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
@@ -4128,7 +4125,7 @@
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
@@ -4138,7 +4135,7 @@
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.2">
@@ -4148,7 +4145,7 @@
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
@@ -4158,7 +4155,7 @@
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.2">
@@ -4168,7 +4165,7 @@
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.2">
@@ -4178,7 +4175,7 @@
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.2">
@@ -4188,7 +4185,7 @@
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.2">
@@ -4198,7 +4195,7 @@
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.2">
@@ -4208,7 +4205,7 @@
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">
@@ -4218,7 +4215,7 @@
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.2">
@@ -4228,7 +4225,7 @@
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.2">
@@ -4238,7 +4235,7 @@
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
@@ -4248,7 +4245,7 @@
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
@@ -4258,7 +4255,7 @@
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.2">
@@ -4268,7 +4265,7 @@
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.2">
@@ -4278,7 +4275,7 @@
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
@@ -4288,7 +4285,7 @@
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.2">
@@ -4298,7 +4295,7 @@
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
@@ -4308,7 +4305,7 @@
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.2">
@@ -4318,7 +4315,7 @@
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.2">
@@ -4328,7 +4325,7 @@
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.2">
@@ -4338,7 +4335,7 @@
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.2">
@@ -4348,7 +4345,7 @@
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.2">
@@ -4358,7 +4355,7 @@
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.2">
@@ -4513,7 +4510,7 @@
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.2">
@@ -4523,7 +4520,7 @@
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.2">
@@ -4533,7 +4530,7 @@
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.2">
@@ -4543,7 +4540,7 @@
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.2">
@@ -4553,7 +4550,7 @@
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.2">
@@ -4563,7 +4560,7 @@
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.2">
@@ -4573,7 +4570,7 @@
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.2">
@@ -4583,7 +4580,7 @@
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.2">
@@ -4597,6 +4594,18 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{924BC353-C18B-E341-A5DC-73D33B76F446}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C5AAF07-546D-E74F-852A-BFCA7F62F822}">
   <dimension ref="A1:AN78"/>
   <sheetViews>

</xml_diff>